<commit_message>
fix crafting objects json
</commit_message>
<xml_diff>
--- a/crafting/Excel Files/Endless Legend - Crafting Tables.xlsx
+++ b/crafting/Excel Files/Endless Legend - Crafting Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZiCold\YandexDisk\TRPGs - Numenera\zicold.github.io\crafting\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87EED771-2E57-457D-AD2F-1AEF361185FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48EB2811-82AD-4A1D-AF93-CD6AAF0D7C2B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="682" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="682" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Salvaging Iotum Table" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1226" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="503">
   <si>
     <t>Iotum</t>
   </si>
@@ -1568,6 +1568,12 @@
   </si>
   <si>
     <t>Common Objects</t>
+  </si>
+  <si>
+    <t>ALARM TOWER</t>
+  </si>
+  <si>
+    <t>This plan produces a 3-foot (1 m) diameter crystal sphere fixed atop a metallic mast that reaches 50 feet (15 m) into the air. It also produces a linked, handheld device with a control surface. The alarm tower monitors along a circumference up to a very long distance away from the tower in all directions. The tower notifes the holder of the handheld device if it detects unusual motion, behavior associated with attempts at stealth, or attempts at crossing the circumference that haven't been previously cleared by the builder (for example, normal traffic on a road or through a gate would probably be cleared by the builder). The alarm tower could be set to scan for different criteria, such as the appearance of a certain kind of creature or even a specific individual. Such a device modifes a community's rank by +1 for tasks related to perception. The wielder of an alarm tower's control device can cause the tower to emit an audible alarm either manually or as an automatic response to what it is set to watch for.</t>
   </si>
 </sst>
 </file>
@@ -4146,7 +4152,7 @@
   <dimension ref="A1:N123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -8397,7 +8403,1471 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:F72"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D69" sqref="D69"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" style="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="113.85546875" style="23" customWidth="1"/>
+    <col min="5" max="5" width="44.42578125" style="48" customWidth="1"/>
+    <col min="6" max="6" width="51.5703125" style="48" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A1" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>417</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="135">
+      <c r="A2" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>501</v>
+      </c>
+      <c r="C2" s="26">
+        <v>5</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>502</v>
+      </c>
+      <c r="E2" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30">
+      <c r="A3" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="26">
+        <v>3</v>
+      </c>
+      <c r="D3" s="46" t="s">
+        <v>305</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="47" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="45">
+      <c r="A4" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="26">
+        <v>5</v>
+      </c>
+      <c r="D4" s="46" t="s">
+        <v>306</v>
+      </c>
+      <c r="E4" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="47" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="90">
+      <c r="A5" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="26">
+        <v>9</v>
+      </c>
+      <c r="D5" s="46" t="s">
+        <v>307</v>
+      </c>
+      <c r="E5" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="47" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="195">
+      <c r="A6" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="26">
+        <v>7</v>
+      </c>
+      <c r="D6" s="46" t="s">
+        <v>308</v>
+      </c>
+      <c r="E6" s="64" t="s">
+        <v>404</v>
+      </c>
+      <c r="F6" s="47" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="60">
+      <c r="A7" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="26">
+        <v>4</v>
+      </c>
+      <c r="D7" s="46" t="s">
+        <v>309</v>
+      </c>
+      <c r="E7" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="47" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="60">
+      <c r="A8" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="26">
+        <v>3</v>
+      </c>
+      <c r="D8" s="46" t="s">
+        <v>310</v>
+      </c>
+      <c r="E8" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="47" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="60">
+      <c r="A9" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="26">
+        <v>1</v>
+      </c>
+      <c r="D9" s="46" t="s">
+        <v>311</v>
+      </c>
+      <c r="E9" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="47" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="60">
+      <c r="A10" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="26">
+        <v>1</v>
+      </c>
+      <c r="D10" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="E10" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="47" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="60">
+      <c r="A11" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" s="26">
+        <v>9</v>
+      </c>
+      <c r="D11" s="46" t="s">
+        <v>312</v>
+      </c>
+      <c r="E11" s="64" t="s">
+        <v>405</v>
+      </c>
+      <c r="F11" s="47" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="75">
+      <c r="A12" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="26">
+        <v>9</v>
+      </c>
+      <c r="D12" s="46" t="s">
+        <v>313</v>
+      </c>
+      <c r="E12" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="47" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="90">
+      <c r="A13" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="45" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="26">
+        <v>8</v>
+      </c>
+      <c r="D13" s="46" t="s">
+        <v>314</v>
+      </c>
+      <c r="E13" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="47" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="120">
+      <c r="A14" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="26">
+        <v>7</v>
+      </c>
+      <c r="D14" s="46" t="s">
+        <v>315</v>
+      </c>
+      <c r="E14" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="47" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="60">
+      <c r="A15" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="26">
+        <v>6</v>
+      </c>
+      <c r="D15" s="46" t="s">
+        <v>316</v>
+      </c>
+      <c r="E15" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="47" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="90">
+      <c r="A16" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="C16" s="26">
+        <v>8</v>
+      </c>
+      <c r="D16" s="46" t="s">
+        <v>317</v>
+      </c>
+      <c r="E16" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="47" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="90">
+      <c r="A17" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="45" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="26">
+        <v>2</v>
+      </c>
+      <c r="D17" s="46" t="s">
+        <v>318</v>
+      </c>
+      <c r="E17" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="47" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="45">
+      <c r="A18" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" s="26">
+        <v>6</v>
+      </c>
+      <c r="D18" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="E18" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="47" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="105">
+      <c r="A19" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" s="26">
+        <v>4</v>
+      </c>
+      <c r="D19" s="46" t="s">
+        <v>319</v>
+      </c>
+      <c r="E19" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="47" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="45">
+      <c r="A20" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="C20" s="26">
+        <v>7</v>
+      </c>
+      <c r="D20" s="46" t="s">
+        <v>320</v>
+      </c>
+      <c r="E20" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="47" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="60">
+      <c r="A21" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21" s="26">
+        <v>9</v>
+      </c>
+      <c r="D21" s="46" t="s">
+        <v>321</v>
+      </c>
+      <c r="E21" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="47" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="60">
+      <c r="A22" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="45" t="s">
+        <v>127</v>
+      </c>
+      <c r="C22" s="26">
+        <v>2</v>
+      </c>
+      <c r="D22" s="46" t="s">
+        <v>322</v>
+      </c>
+      <c r="E22" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="47" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="75">
+      <c r="A23" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="C23" s="26">
+        <v>8</v>
+      </c>
+      <c r="D23" s="46" t="s">
+        <v>323</v>
+      </c>
+      <c r="E23" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="47" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="60">
+      <c r="A24" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="C24" s="26">
+        <v>4</v>
+      </c>
+      <c r="D24" s="46" t="s">
+        <v>324</v>
+      </c>
+      <c r="E24" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="47" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="45">
+      <c r="A25" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" s="45" t="s">
+        <v>132</v>
+      </c>
+      <c r="C25" s="26">
+        <v>9</v>
+      </c>
+      <c r="D25" s="46" t="s">
+        <v>325</v>
+      </c>
+      <c r="E25" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="47" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="60">
+      <c r="A26" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="C26" s="26">
+        <v>6</v>
+      </c>
+      <c r="D26" s="46" t="s">
+        <v>326</v>
+      </c>
+      <c r="E26" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="47" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="60">
+      <c r="A27" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" s="45" t="s">
+        <v>135</v>
+      </c>
+      <c r="C27" s="26">
+        <v>3</v>
+      </c>
+      <c r="D27" s="46" t="s">
+        <v>136</v>
+      </c>
+      <c r="E27" s="64" t="s">
+        <v>406</v>
+      </c>
+      <c r="F27" s="47" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="60">
+      <c r="A28" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" s="45" t="s">
+        <v>137</v>
+      </c>
+      <c r="C28" s="26">
+        <v>2</v>
+      </c>
+      <c r="D28" s="46" t="s">
+        <v>327</v>
+      </c>
+      <c r="E28" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="47" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B29" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="C29" s="26">
+        <v>5</v>
+      </c>
+      <c r="D29" s="46" t="s">
+        <v>140</v>
+      </c>
+      <c r="E29" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F29" s="47" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="45">
+      <c r="A30" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="C30" s="26">
+        <v>8</v>
+      </c>
+      <c r="D30" s="46" t="s">
+        <v>328</v>
+      </c>
+      <c r="E30" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F30" s="47" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="75">
+      <c r="A31" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="45" t="s">
+        <v>144</v>
+      </c>
+      <c r="C31" s="26">
+        <v>3</v>
+      </c>
+      <c r="D31" s="63" t="s">
+        <v>329</v>
+      </c>
+      <c r="E31" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" s="47" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="120">
+      <c r="A32" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" s="45" t="s">
+        <v>146</v>
+      </c>
+      <c r="C32" s="26">
+        <v>5</v>
+      </c>
+      <c r="D32" s="46" t="s">
+        <v>330</v>
+      </c>
+      <c r="E32" s="64" t="s">
+        <v>405</v>
+      </c>
+      <c r="F32" s="47" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="90">
+      <c r="A33" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" s="45" t="s">
+        <v>148</v>
+      </c>
+      <c r="C33" s="26">
+        <v>8</v>
+      </c>
+      <c r="D33" s="46" t="s">
+        <v>331</v>
+      </c>
+      <c r="E33" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F33" s="47" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="45">
+      <c r="A34" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" s="45" t="s">
+        <v>149</v>
+      </c>
+      <c r="C34" s="26">
+        <v>1</v>
+      </c>
+      <c r="D34" s="46" t="s">
+        <v>150</v>
+      </c>
+      <c r="E34" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" s="47" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="60">
+      <c r="A35" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" s="45" t="s">
+        <v>153</v>
+      </c>
+      <c r="C35" s="26">
+        <v>6</v>
+      </c>
+      <c r="D35" s="46" t="s">
+        <v>333</v>
+      </c>
+      <c r="E35" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F35" s="47" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="45">
+      <c r="A36" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B36" s="45" t="s">
+        <v>152</v>
+      </c>
+      <c r="C36" s="26">
+        <v>3</v>
+      </c>
+      <c r="D36" s="46" t="s">
+        <v>332</v>
+      </c>
+      <c r="E36" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F36" s="47" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="240">
+      <c r="A37" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B37" s="45" t="s">
+        <v>154</v>
+      </c>
+      <c r="C37" s="26">
+        <v>4</v>
+      </c>
+      <c r="D37" s="46" t="s">
+        <v>334</v>
+      </c>
+      <c r="E37" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F37" s="47" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="75">
+      <c r="A38" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B38" s="45" t="s">
+        <v>155</v>
+      </c>
+      <c r="C38" s="26">
+        <v>4</v>
+      </c>
+      <c r="D38" s="46" t="s">
+        <v>335</v>
+      </c>
+      <c r="E38" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F38" s="47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="75">
+      <c r="A39" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" s="45" t="s">
+        <v>156</v>
+      </c>
+      <c r="C39" s="26">
+        <v>2</v>
+      </c>
+      <c r="D39" s="46" t="s">
+        <v>336</v>
+      </c>
+      <c r="E39" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F39" s="47" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="90">
+      <c r="A40" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B40" s="45" t="s">
+        <v>158</v>
+      </c>
+      <c r="C40" s="26">
+        <v>9</v>
+      </c>
+      <c r="D40" s="46" t="s">
+        <v>337</v>
+      </c>
+      <c r="E40" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F40" s="47" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="60">
+      <c r="A41" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" s="45" t="s">
+        <v>160</v>
+      </c>
+      <c r="C41" s="26">
+        <v>2</v>
+      </c>
+      <c r="D41" s="46" t="s">
+        <v>338</v>
+      </c>
+      <c r="E41" s="65" t="s">
+        <v>407</v>
+      </c>
+      <c r="F41" s="47" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="45">
+      <c r="A42" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B42" s="45" t="s">
+        <v>161</v>
+      </c>
+      <c r="C42" s="26">
+        <v>2</v>
+      </c>
+      <c r="D42" s="46" t="s">
+        <v>339</v>
+      </c>
+      <c r="E42" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F42" s="47" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="60">
+      <c r="A43" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B43" s="45" t="s">
+        <v>163</v>
+      </c>
+      <c r="C43" s="26">
+        <v>7</v>
+      </c>
+      <c r="D43" s="46" t="s">
+        <v>340</v>
+      </c>
+      <c r="E43" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F43" s="47" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="75">
+      <c r="A44" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B44" s="45" t="s">
+        <v>165</v>
+      </c>
+      <c r="C44" s="26">
+        <v>7</v>
+      </c>
+      <c r="D44" s="46" t="s">
+        <v>341</v>
+      </c>
+      <c r="E44" s="65" t="s">
+        <v>408</v>
+      </c>
+      <c r="F44" s="47" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="45">
+      <c r="A45" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" s="45" t="s">
+        <v>167</v>
+      </c>
+      <c r="C45" s="26">
+        <v>5</v>
+      </c>
+      <c r="D45" s="46" t="s">
+        <v>342</v>
+      </c>
+      <c r="E45" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F45" s="47" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="90">
+      <c r="A46" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B46" s="45" t="s">
+        <v>168</v>
+      </c>
+      <c r="C46" s="26">
+        <v>2</v>
+      </c>
+      <c r="D46" s="46" t="s">
+        <v>343</v>
+      </c>
+      <c r="E46" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F46" s="47" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="75">
+      <c r="A47" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B47" s="45" t="s">
+        <v>169</v>
+      </c>
+      <c r="C47" s="26">
+        <v>6</v>
+      </c>
+      <c r="D47" s="46" t="s">
+        <v>344</v>
+      </c>
+      <c r="E47" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F47" s="47" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="45">
+      <c r="A48" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B48" s="45" t="s">
+        <v>170</v>
+      </c>
+      <c r="C48" s="26">
+        <v>5</v>
+      </c>
+      <c r="D48" s="46" t="s">
+        <v>345</v>
+      </c>
+      <c r="E48" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F48" s="47" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="120">
+      <c r="A49" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B49" s="45" t="s">
+        <v>171</v>
+      </c>
+      <c r="C49" s="26">
+        <v>5</v>
+      </c>
+      <c r="D49" s="46" t="s">
+        <v>346</v>
+      </c>
+      <c r="E49" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F49" s="47" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="75">
+      <c r="A50" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" s="45" t="s">
+        <v>172</v>
+      </c>
+      <c r="C50" s="26">
+        <v>6</v>
+      </c>
+      <c r="D50" s="46" t="s">
+        <v>347</v>
+      </c>
+      <c r="E50" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F50" s="47" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="150">
+      <c r="A51" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B51" s="45" t="s">
+        <v>173</v>
+      </c>
+      <c r="C51" s="26">
+        <v>10</v>
+      </c>
+      <c r="D51" s="46" t="s">
+        <v>348</v>
+      </c>
+      <c r="E51" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F51" s="47" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="150">
+      <c r="A52" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B52" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="C52" s="26">
+        <v>10</v>
+      </c>
+      <c r="D52" s="46" t="s">
+        <v>349</v>
+      </c>
+      <c r="E52" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F52" s="47" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="90">
+      <c r="A53" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="C53" s="26">
+        <v>2</v>
+      </c>
+      <c r="D53" s="46" t="s">
+        <v>350</v>
+      </c>
+      <c r="E53" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F53" s="47" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="45">
+      <c r="A54" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B54" s="45" t="s">
+        <v>178</v>
+      </c>
+      <c r="C54" s="26">
+        <v>4</v>
+      </c>
+      <c r="D54" s="46" t="s">
+        <v>351</v>
+      </c>
+      <c r="E54" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F54" s="47" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="75">
+      <c r="A55" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B55" s="45" t="s">
+        <v>179</v>
+      </c>
+      <c r="C55" s="26">
+        <v>4</v>
+      </c>
+      <c r="D55" s="46" t="s">
+        <v>352</v>
+      </c>
+      <c r="E55" s="65" t="s">
+        <v>409</v>
+      </c>
+      <c r="F55" s="47" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="165">
+      <c r="A56" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B56" s="45" t="s">
+        <v>180</v>
+      </c>
+      <c r="C56" s="26">
+        <v>4</v>
+      </c>
+      <c r="D56" s="46" t="s">
+        <v>353</v>
+      </c>
+      <c r="E56" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F56" s="47" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="75">
+      <c r="A57" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B57" s="45" t="s">
+        <v>181</v>
+      </c>
+      <c r="C57" s="26">
+        <v>4</v>
+      </c>
+      <c r="D57" s="46" t="s">
+        <v>354</v>
+      </c>
+      <c r="E57" s="65" t="s">
+        <v>411</v>
+      </c>
+      <c r="F57" s="47" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="75">
+      <c r="A58" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B58" s="45" t="s">
+        <v>182</v>
+      </c>
+      <c r="C58" s="26">
+        <v>5</v>
+      </c>
+      <c r="D58" s="46" t="s">
+        <v>355</v>
+      </c>
+      <c r="E58" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F58" s="47" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="75">
+      <c r="A59" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B59" s="45" t="s">
+        <v>183</v>
+      </c>
+      <c r="C59" s="26">
+        <v>2</v>
+      </c>
+      <c r="D59" s="46" t="s">
+        <v>356</v>
+      </c>
+      <c r="E59" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F59" s="47" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="75">
+      <c r="A60" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B60" s="45" t="s">
+        <v>185</v>
+      </c>
+      <c r="C60" s="26">
+        <v>7</v>
+      </c>
+      <c r="D60" s="46" t="s">
+        <v>357</v>
+      </c>
+      <c r="E60" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F60" s="47" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="60">
+      <c r="A61" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B61" s="45" t="s">
+        <v>187</v>
+      </c>
+      <c r="C61" s="26">
+        <v>4</v>
+      </c>
+      <c r="D61" s="46" t="s">
+        <v>358</v>
+      </c>
+      <c r="E61" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F61" s="47" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="75">
+      <c r="A62" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B62" s="45" t="s">
+        <v>188</v>
+      </c>
+      <c r="C62" s="26">
+        <v>6</v>
+      </c>
+      <c r="D62" s="46" t="s">
+        <v>359</v>
+      </c>
+      <c r="E62" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F62" s="47" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="45">
+      <c r="A63" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B63" s="45" t="s">
+        <v>189</v>
+      </c>
+      <c r="C63" s="26">
+        <v>5</v>
+      </c>
+      <c r="D63" s="46" t="s">
+        <v>360</v>
+      </c>
+      <c r="E63" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F63" s="47" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="90">
+      <c r="A64" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B64" s="45" t="s">
+        <v>190</v>
+      </c>
+      <c r="C64" s="26">
+        <v>7</v>
+      </c>
+      <c r="D64" s="46" t="s">
+        <v>361</v>
+      </c>
+      <c r="E64" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F64" s="47" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="45">
+      <c r="A65" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B65" s="45" t="s">
+        <v>191</v>
+      </c>
+      <c r="C65" s="26">
+        <v>2</v>
+      </c>
+      <c r="D65" s="46" t="s">
+        <v>362</v>
+      </c>
+      <c r="E65" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F65" s="47" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="60">
+      <c r="A66" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B66" s="45" t="s">
+        <v>192</v>
+      </c>
+      <c r="C66" s="26">
+        <v>5</v>
+      </c>
+      <c r="D66" s="46" t="s">
+        <v>363</v>
+      </c>
+      <c r="E66" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F66" s="47" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="30">
+      <c r="A67" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B67" s="45" t="s">
+        <v>193</v>
+      </c>
+      <c r="C67" s="26">
+        <v>1</v>
+      </c>
+      <c r="D67" s="46" t="s">
+        <v>194</v>
+      </c>
+      <c r="E67" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F67" s="47" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="60">
+      <c r="A68" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B68" s="45" t="s">
+        <v>195</v>
+      </c>
+      <c r="C68" s="26">
+        <v>5</v>
+      </c>
+      <c r="D68" s="46" t="s">
+        <v>364</v>
+      </c>
+      <c r="E68" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F68" s="47" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="45">
+      <c r="A69" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B69" s="45" t="s">
+        <v>199</v>
+      </c>
+      <c r="C69" s="26">
+        <v>8</v>
+      </c>
+      <c r="D69" s="46" t="s">
+        <v>367</v>
+      </c>
+      <c r="E69" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F69" s="47" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="90">
+      <c r="A70" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B70" s="45" t="s">
+        <v>197</v>
+      </c>
+      <c r="C70" s="26">
+        <v>2</v>
+      </c>
+      <c r="D70" s="46" t="s">
+        <v>365</v>
+      </c>
+      <c r="E70" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F70" s="47" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="45">
+      <c r="A71" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B71" s="45" t="s">
+        <v>198</v>
+      </c>
+      <c r="C71" s="26">
+        <v>5</v>
+      </c>
+      <c r="D71" s="46" t="s">
+        <v>366</v>
+      </c>
+      <c r="E71" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F71" s="47" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="90">
+      <c r="A72" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B72" s="45" t="s">
+        <v>201</v>
+      </c>
+      <c r="C72" s="26">
+        <v>6</v>
+      </c>
+      <c r="D72" s="46" t="s">
+        <v>368</v>
+      </c>
+      <c r="E72" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F72" s="47" t="s">
+        <v>202</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -8434,1450 +9904,6 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30">
-      <c r="A2" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B2" s="45" t="s">
-        <v>90</v>
-      </c>
-      <c r="C2" s="26">
-        <v>3</v>
-      </c>
-      <c r="D2" s="46" t="s">
-        <v>305</v>
-      </c>
-      <c r="E2" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="47" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="45">
-      <c r="A3" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B3" s="45" t="s">
-        <v>92</v>
-      </c>
-      <c r="C3" s="26">
-        <v>5</v>
-      </c>
-      <c r="D3" s="46" t="s">
-        <v>306</v>
-      </c>
-      <c r="E3" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="47" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="90">
-      <c r="A4" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B4" s="45" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4" s="26">
-        <v>9</v>
-      </c>
-      <c r="D4" s="46" t="s">
-        <v>307</v>
-      </c>
-      <c r="E4" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="47" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="195">
-      <c r="A5" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B5" s="45" t="s">
-        <v>96</v>
-      </c>
-      <c r="C5" s="26">
-        <v>7</v>
-      </c>
-      <c r="D5" s="46" t="s">
-        <v>308</v>
-      </c>
-      <c r="E5" s="64" t="s">
-        <v>404</v>
-      </c>
-      <c r="F5" s="47" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="60">
-      <c r="A6" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B6" s="45" t="s">
-        <v>98</v>
-      </c>
-      <c r="C6" s="26">
-        <v>4</v>
-      </c>
-      <c r="D6" s="46" t="s">
-        <v>309</v>
-      </c>
-      <c r="E6" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" s="47" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="60">
-      <c r="A7" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B7" s="45" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" s="26">
-        <v>3</v>
-      </c>
-      <c r="D7" s="46" t="s">
-        <v>310</v>
-      </c>
-      <c r="E7" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="47" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="60">
-      <c r="A8" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B8" s="45" t="s">
-        <v>105</v>
-      </c>
-      <c r="C8" s="26">
-        <v>1</v>
-      </c>
-      <c r="D8" s="46" t="s">
-        <v>311</v>
-      </c>
-      <c r="E8" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="47" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="60">
-      <c r="A9" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B9" s="45" t="s">
-        <v>102</v>
-      </c>
-      <c r="C9" s="26">
-        <v>1</v>
-      </c>
-      <c r="D9" s="46" t="s">
-        <v>103</v>
-      </c>
-      <c r="E9" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="47" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="60">
-      <c r="A10" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B10" s="45" t="s">
-        <v>106</v>
-      </c>
-      <c r="C10" s="26">
-        <v>9</v>
-      </c>
-      <c r="D10" s="46" t="s">
-        <v>312</v>
-      </c>
-      <c r="E10" s="64" t="s">
-        <v>405</v>
-      </c>
-      <c r="F10" s="47" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="75">
-      <c r="A11" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B11" s="45" t="s">
-        <v>108</v>
-      </c>
-      <c r="C11" s="26">
-        <v>9</v>
-      </c>
-      <c r="D11" s="46" t="s">
-        <v>313</v>
-      </c>
-      <c r="E11" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" s="47" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="90">
-      <c r="A12" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B12" s="45" t="s">
-        <v>110</v>
-      </c>
-      <c r="C12" s="26">
-        <v>8</v>
-      </c>
-      <c r="D12" s="46" t="s">
-        <v>314</v>
-      </c>
-      <c r="E12" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="47" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="120">
-      <c r="A13" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B13" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="C13" s="26">
-        <v>7</v>
-      </c>
-      <c r="D13" s="46" t="s">
-        <v>315</v>
-      </c>
-      <c r="E13" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="47" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="60">
-      <c r="A14" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B14" s="45" t="s">
-        <v>114</v>
-      </c>
-      <c r="C14" s="26">
-        <v>6</v>
-      </c>
-      <c r="D14" s="46" t="s">
-        <v>316</v>
-      </c>
-      <c r="E14" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="47" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="90">
-      <c r="A15" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B15" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="C15" s="26">
-        <v>8</v>
-      </c>
-      <c r="D15" s="46" t="s">
-        <v>317</v>
-      </c>
-      <c r="E15" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15" s="47" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="90">
-      <c r="A16" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B16" s="45" t="s">
-        <v>118</v>
-      </c>
-      <c r="C16" s="26">
-        <v>2</v>
-      </c>
-      <c r="D16" s="46" t="s">
-        <v>318</v>
-      </c>
-      <c r="E16" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="47" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="45">
-      <c r="A17" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B17" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="C17" s="26">
-        <v>6</v>
-      </c>
-      <c r="D17" s="46" t="s">
-        <v>120</v>
-      </c>
-      <c r="E17" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F17" s="47" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="105">
-      <c r="A18" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B18" s="45" t="s">
-        <v>122</v>
-      </c>
-      <c r="C18" s="26">
-        <v>4</v>
-      </c>
-      <c r="D18" s="46" t="s">
-        <v>319</v>
-      </c>
-      <c r="E18" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F18" s="47" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="45">
-      <c r="A19" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B19" s="45" t="s">
-        <v>124</v>
-      </c>
-      <c r="C19" s="26">
-        <v>7</v>
-      </c>
-      <c r="D19" s="46" t="s">
-        <v>320</v>
-      </c>
-      <c r="E19" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F19" s="47" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="60">
-      <c r="A20" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B20" s="45" t="s">
-        <v>126</v>
-      </c>
-      <c r="C20" s="26">
-        <v>9</v>
-      </c>
-      <c r="D20" s="46" t="s">
-        <v>321</v>
-      </c>
-      <c r="E20" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20" s="47" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="60">
-      <c r="A21" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B21" s="45" t="s">
-        <v>127</v>
-      </c>
-      <c r="C21" s="26">
-        <v>2</v>
-      </c>
-      <c r="D21" s="46" t="s">
-        <v>322</v>
-      </c>
-      <c r="E21" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" s="47" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="75">
-      <c r="A22" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B22" s="45" t="s">
-        <v>129</v>
-      </c>
-      <c r="C22" s="26">
-        <v>8</v>
-      </c>
-      <c r="D22" s="46" t="s">
-        <v>323</v>
-      </c>
-      <c r="E22" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F22" s="47" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="60">
-      <c r="A23" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B23" s="45" t="s">
-        <v>131</v>
-      </c>
-      <c r="C23" s="26">
-        <v>4</v>
-      </c>
-      <c r="D23" s="46" t="s">
-        <v>324</v>
-      </c>
-      <c r="E23" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F23" s="47" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="45">
-      <c r="A24" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B24" s="45" t="s">
-        <v>132</v>
-      </c>
-      <c r="C24" s="26">
-        <v>9</v>
-      </c>
-      <c r="D24" s="46" t="s">
-        <v>325</v>
-      </c>
-      <c r="E24" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="47" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="60">
-      <c r="A25" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B25" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="C25" s="26">
-        <v>6</v>
-      </c>
-      <c r="D25" s="46" t="s">
-        <v>326</v>
-      </c>
-      <c r="E25" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25" s="47" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="60">
-      <c r="A26" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B26" s="45" t="s">
-        <v>135</v>
-      </c>
-      <c r="C26" s="26">
-        <v>3</v>
-      </c>
-      <c r="D26" s="46" t="s">
-        <v>136</v>
-      </c>
-      <c r="E26" s="64" t="s">
-        <v>406</v>
-      </c>
-      <c r="F26" s="47" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="60">
-      <c r="A27" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B27" s="45" t="s">
-        <v>137</v>
-      </c>
-      <c r="C27" s="26">
-        <v>2</v>
-      </c>
-      <c r="D27" s="46" t="s">
-        <v>327</v>
-      </c>
-      <c r="E27" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" s="47" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B28" s="45" t="s">
-        <v>139</v>
-      </c>
-      <c r="C28" s="26">
-        <v>5</v>
-      </c>
-      <c r="D28" s="46" t="s">
-        <v>140</v>
-      </c>
-      <c r="E28" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F28" s="47" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="45">
-      <c r="A29" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B29" s="45" t="s">
-        <v>142</v>
-      </c>
-      <c r="C29" s="26">
-        <v>8</v>
-      </c>
-      <c r="D29" s="46" t="s">
-        <v>328</v>
-      </c>
-      <c r="E29" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F29" s="47" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="75">
-      <c r="A30" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B30" s="45" t="s">
-        <v>144</v>
-      </c>
-      <c r="C30" s="26">
-        <v>3</v>
-      </c>
-      <c r="D30" s="63" t="s">
-        <v>329</v>
-      </c>
-      <c r="E30" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F30" s="47" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="120">
-      <c r="A31" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B31" s="45" t="s">
-        <v>146</v>
-      </c>
-      <c r="C31" s="26">
-        <v>5</v>
-      </c>
-      <c r="D31" s="46" t="s">
-        <v>330</v>
-      </c>
-      <c r="E31" s="64" t="s">
-        <v>405</v>
-      </c>
-      <c r="F31" s="47" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="90">
-      <c r="A32" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B32" s="45" t="s">
-        <v>148</v>
-      </c>
-      <c r="C32" s="26">
-        <v>8</v>
-      </c>
-      <c r="D32" s="46" t="s">
-        <v>331</v>
-      </c>
-      <c r="E32" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F32" s="47" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="45">
-      <c r="A33" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B33" s="45" t="s">
-        <v>149</v>
-      </c>
-      <c r="C33" s="26">
-        <v>1</v>
-      </c>
-      <c r="D33" s="46" t="s">
-        <v>150</v>
-      </c>
-      <c r="E33" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F33" s="47" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="60">
-      <c r="A34" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B34" s="45" t="s">
-        <v>153</v>
-      </c>
-      <c r="C34" s="26">
-        <v>6</v>
-      </c>
-      <c r="D34" s="46" t="s">
-        <v>333</v>
-      </c>
-      <c r="E34" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F34" s="47" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="45">
-      <c r="A35" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B35" s="45" t="s">
-        <v>152</v>
-      </c>
-      <c r="C35" s="26">
-        <v>3</v>
-      </c>
-      <c r="D35" s="46" t="s">
-        <v>332</v>
-      </c>
-      <c r="E35" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F35" s="47" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="240">
-      <c r="A36" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B36" s="45" t="s">
-        <v>154</v>
-      </c>
-      <c r="C36" s="26">
-        <v>4</v>
-      </c>
-      <c r="D36" s="46" t="s">
-        <v>334</v>
-      </c>
-      <c r="E36" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F36" s="47" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="75">
-      <c r="A37" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B37" s="45" t="s">
-        <v>155</v>
-      </c>
-      <c r="C37" s="26">
-        <v>4</v>
-      </c>
-      <c r="D37" s="46" t="s">
-        <v>335</v>
-      </c>
-      <c r="E37" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F37" s="47" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="75">
-      <c r="A38" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B38" s="45" t="s">
-        <v>156</v>
-      </c>
-      <c r="C38" s="26">
-        <v>2</v>
-      </c>
-      <c r="D38" s="46" t="s">
-        <v>336</v>
-      </c>
-      <c r="E38" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F38" s="47" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="90">
-      <c r="A39" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B39" s="45" t="s">
-        <v>158</v>
-      </c>
-      <c r="C39" s="26">
-        <v>9</v>
-      </c>
-      <c r="D39" s="46" t="s">
-        <v>337</v>
-      </c>
-      <c r="E39" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F39" s="47" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="60">
-      <c r="A40" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B40" s="45" t="s">
-        <v>160</v>
-      </c>
-      <c r="C40" s="26">
-        <v>2</v>
-      </c>
-      <c r="D40" s="46" t="s">
-        <v>338</v>
-      </c>
-      <c r="E40" s="65" t="s">
-        <v>407</v>
-      </c>
-      <c r="F40" s="47" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="45">
-      <c r="A41" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B41" s="45" t="s">
-        <v>161</v>
-      </c>
-      <c r="C41" s="26">
-        <v>2</v>
-      </c>
-      <c r="D41" s="46" t="s">
-        <v>339</v>
-      </c>
-      <c r="E41" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F41" s="47" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="60">
-      <c r="A42" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B42" s="45" t="s">
-        <v>163</v>
-      </c>
-      <c r="C42" s="26">
-        <v>7</v>
-      </c>
-      <c r="D42" s="46" t="s">
-        <v>340</v>
-      </c>
-      <c r="E42" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F42" s="47" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="75">
-      <c r="A43" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B43" s="45" t="s">
-        <v>165</v>
-      </c>
-      <c r="C43" s="26">
-        <v>7</v>
-      </c>
-      <c r="D43" s="46" t="s">
-        <v>341</v>
-      </c>
-      <c r="E43" s="65" t="s">
-        <v>408</v>
-      </c>
-      <c r="F43" s="47" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="45">
-      <c r="A44" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B44" s="45" t="s">
-        <v>167</v>
-      </c>
-      <c r="C44" s="26">
-        <v>5</v>
-      </c>
-      <c r="D44" s="46" t="s">
-        <v>342</v>
-      </c>
-      <c r="E44" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F44" s="47" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="90">
-      <c r="A45" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B45" s="45" t="s">
-        <v>168</v>
-      </c>
-      <c r="C45" s="26">
-        <v>2</v>
-      </c>
-      <c r="D45" s="46" t="s">
-        <v>343</v>
-      </c>
-      <c r="E45" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F45" s="47" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="75">
-      <c r="A46" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B46" s="45" t="s">
-        <v>169</v>
-      </c>
-      <c r="C46" s="26">
-        <v>6</v>
-      </c>
-      <c r="D46" s="46" t="s">
-        <v>344</v>
-      </c>
-      <c r="E46" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F46" s="47" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="45">
-      <c r="A47" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B47" s="45" t="s">
-        <v>170</v>
-      </c>
-      <c r="C47" s="26">
-        <v>5</v>
-      </c>
-      <c r="D47" s="46" t="s">
-        <v>345</v>
-      </c>
-      <c r="E47" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F47" s="47" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="120">
-      <c r="A48" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B48" s="45" t="s">
-        <v>171</v>
-      </c>
-      <c r="C48" s="26">
-        <v>5</v>
-      </c>
-      <c r="D48" s="46" t="s">
-        <v>346</v>
-      </c>
-      <c r="E48" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F48" s="47" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="75">
-      <c r="A49" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B49" s="45" t="s">
-        <v>172</v>
-      </c>
-      <c r="C49" s="26">
-        <v>6</v>
-      </c>
-      <c r="D49" s="46" t="s">
-        <v>347</v>
-      </c>
-      <c r="E49" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F49" s="47" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="150">
-      <c r="A50" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B50" s="45" t="s">
-        <v>173</v>
-      </c>
-      <c r="C50" s="26">
-        <v>10</v>
-      </c>
-      <c r="D50" s="46" t="s">
-        <v>348</v>
-      </c>
-      <c r="E50" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F50" s="47" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="150">
-      <c r="A51" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B51" s="45" t="s">
-        <v>175</v>
-      </c>
-      <c r="C51" s="26">
-        <v>10</v>
-      </c>
-      <c r="D51" s="46" t="s">
-        <v>349</v>
-      </c>
-      <c r="E51" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F51" s="47" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="90">
-      <c r="A52" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B52" s="45" t="s">
-        <v>177</v>
-      </c>
-      <c r="C52" s="26">
-        <v>2</v>
-      </c>
-      <c r="D52" s="46" t="s">
-        <v>350</v>
-      </c>
-      <c r="E52" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F52" s="47" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="45">
-      <c r="A53" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B53" s="45" t="s">
-        <v>178</v>
-      </c>
-      <c r="C53" s="26">
-        <v>4</v>
-      </c>
-      <c r="D53" s="46" t="s">
-        <v>351</v>
-      </c>
-      <c r="E53" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F53" s="47" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="75">
-      <c r="A54" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B54" s="45" t="s">
-        <v>179</v>
-      </c>
-      <c r="C54" s="26">
-        <v>4</v>
-      </c>
-      <c r="D54" s="46" t="s">
-        <v>352</v>
-      </c>
-      <c r="E54" s="65" t="s">
-        <v>409</v>
-      </c>
-      <c r="F54" s="47" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="165">
-      <c r="A55" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B55" s="45" t="s">
-        <v>180</v>
-      </c>
-      <c r="C55" s="26">
-        <v>4</v>
-      </c>
-      <c r="D55" s="46" t="s">
-        <v>353</v>
-      </c>
-      <c r="E55" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F55" s="47" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="75">
-      <c r="A56" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B56" s="45" t="s">
-        <v>181</v>
-      </c>
-      <c r="C56" s="26">
-        <v>4</v>
-      </c>
-      <c r="D56" s="46" t="s">
-        <v>354</v>
-      </c>
-      <c r="E56" s="65" t="s">
-        <v>411</v>
-      </c>
-      <c r="F56" s="47" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="75">
-      <c r="A57" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B57" s="45" t="s">
-        <v>182</v>
-      </c>
-      <c r="C57" s="26">
-        <v>5</v>
-      </c>
-      <c r="D57" s="46" t="s">
-        <v>355</v>
-      </c>
-      <c r="E57" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F57" s="47" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="75">
-      <c r="A58" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B58" s="45" t="s">
-        <v>183</v>
-      </c>
-      <c r="C58" s="26">
-        <v>2</v>
-      </c>
-      <c r="D58" s="46" t="s">
-        <v>356</v>
-      </c>
-      <c r="E58" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F58" s="47" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="75">
-      <c r="A59" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B59" s="45" t="s">
-        <v>185</v>
-      </c>
-      <c r="C59" s="26">
-        <v>7</v>
-      </c>
-      <c r="D59" s="46" t="s">
-        <v>357</v>
-      </c>
-      <c r="E59" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F59" s="47" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="60">
-      <c r="A60" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B60" s="45" t="s">
-        <v>187</v>
-      </c>
-      <c r="C60" s="26">
-        <v>4</v>
-      </c>
-      <c r="D60" s="46" t="s">
-        <v>358</v>
-      </c>
-      <c r="E60" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F60" s="47" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="75">
-      <c r="A61" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B61" s="45" t="s">
-        <v>188</v>
-      </c>
-      <c r="C61" s="26">
-        <v>6</v>
-      </c>
-      <c r="D61" s="46" t="s">
-        <v>359</v>
-      </c>
-      <c r="E61" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F61" s="47" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="45">
-      <c r="A62" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B62" s="45" t="s">
-        <v>189</v>
-      </c>
-      <c r="C62" s="26">
-        <v>5</v>
-      </c>
-      <c r="D62" s="46" t="s">
-        <v>360</v>
-      </c>
-      <c r="E62" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F62" s="47" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="90">
-      <c r="A63" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B63" s="45" t="s">
-        <v>190</v>
-      </c>
-      <c r="C63" s="26">
-        <v>7</v>
-      </c>
-      <c r="D63" s="46" t="s">
-        <v>361</v>
-      </c>
-      <c r="E63" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F63" s="47" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="45">
-      <c r="A64" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B64" s="45" t="s">
-        <v>191</v>
-      </c>
-      <c r="C64" s="26">
-        <v>2</v>
-      </c>
-      <c r="D64" s="46" t="s">
-        <v>362</v>
-      </c>
-      <c r="E64" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F64" s="47" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="60">
-      <c r="A65" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B65" s="45" t="s">
-        <v>192</v>
-      </c>
-      <c r="C65" s="26">
-        <v>5</v>
-      </c>
-      <c r="D65" s="46" t="s">
-        <v>363</v>
-      </c>
-      <c r="E65" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F65" s="47" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="30">
-      <c r="A66" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B66" s="45" t="s">
-        <v>193</v>
-      </c>
-      <c r="C66" s="26">
-        <v>1</v>
-      </c>
-      <c r="D66" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="E66" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F66" s="47" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="60">
-      <c r="A67" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B67" s="45" t="s">
-        <v>195</v>
-      </c>
-      <c r="C67" s="26">
-        <v>5</v>
-      </c>
-      <c r="D67" s="46" t="s">
-        <v>364</v>
-      </c>
-      <c r="E67" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F67" s="47" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="45">
-      <c r="A68" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B68" s="45" t="s">
-        <v>199</v>
-      </c>
-      <c r="C68" s="26">
-        <v>8</v>
-      </c>
-      <c r="D68" s="46" t="s">
-        <v>367</v>
-      </c>
-      <c r="E68" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F68" s="47" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="90">
-      <c r="A69" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B69" s="45" t="s">
-        <v>197</v>
-      </c>
-      <c r="C69" s="26">
-        <v>2</v>
-      </c>
-      <c r="D69" s="46" t="s">
-        <v>365</v>
-      </c>
-      <c r="E69" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F69" s="47" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="45">
-      <c r="A70" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B70" s="45" t="s">
-        <v>198</v>
-      </c>
-      <c r="C70" s="26">
-        <v>5</v>
-      </c>
-      <c r="D70" s="46" t="s">
-        <v>366</v>
-      </c>
-      <c r="E70" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F70" s="47" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="90">
-      <c r="A71" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B71" s="45" t="s">
-        <v>201</v>
-      </c>
-      <c r="C71" s="26">
-        <v>6</v>
-      </c>
-      <c r="D71" s="46" t="s">
-        <v>368</v>
-      </c>
-      <c r="E71" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F71" s="47" t="s">
-        <v>202</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:F19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="11" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" style="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="113.85546875" style="23" customWidth="1"/>
-    <col min="5" max="5" width="44.42578125" style="48" customWidth="1"/>
-    <col min="6" max="6" width="51.5703125" style="48" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A1" s="39" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="40" t="s">
-        <v>417</v>
-      </c>
-      <c r="D1" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" s="40" t="s">
-        <v>49</v>
-      </c>
-    </row>
     <row r="2" spans="1:6" ht="60">
       <c r="A2" s="49" t="s">
         <v>50</v>
@@ -10251,9 +10277,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>